<commit_message>
hull white 1 factor
</commit_message>
<xml_diff>
--- a/frm/pricing_engine/hull_white/zero_data.xlsx
+++ b/frm/pricing_engine/hull_white/zero_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shasa\Documents\finance_calcs\frm\frm\pricing_engine\hull_white\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E282B6-BFD4-4817-A98C-DC0B6D054753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE243A1-B6BF-4280-AC6B-BA499B7EAA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{79DB474E-5FF9-486E-ACD6-6CA91B488577}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15720" xr2:uid="{79DB474E-5FF9-486E-ACD6-6CA91B488577}"/>
   </bookViews>
   <sheets>
     <sheet name="Strips" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
     <t>years</t>
   </si>
   <si>
-    <t>zero_rates</t>
+    <t>discount_factor</t>
   </si>
   <si>
-    <t>discount_factor</t>
+    <t>zero_rate</t>
   </si>
 </sst>
 </file>
@@ -888,7 +888,7 @@
   <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -902,10 +902,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>